<commit_message>
POL-2962: return cell value when Money parsing fails (#2377)
* POL-2962: return cell value when Money parsing fails

* POL-2962: add check for existence in Money Currency table
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_pricings.xlsx
+++ b/spec/fixtures/files/excel/example_pricings.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjC2NHCw5zZFIFkspl50/u7d8Qskg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mi39H4mgw0hRjZR4E53bDyv1FQwgg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
   <si>
     <t>GROUP_ID</t>
   </si>
@@ -43,18 +43,18 @@
     <t>COUNTRY_DESTINATION</t>
   </si>
   <si>
+    <t>DESTINATION</t>
+  </si>
+  <si>
+    <t>DESTINATION_LOCODE</t>
+  </si>
+  <si>
+    <t>TRANSSHIPMENT</t>
+  </si>
+  <si>
     <t>MOT</t>
   </si>
   <si>
-    <t>DESTINATION</t>
-  </si>
-  <si>
-    <t>DESTINATION_LOCODE</t>
-  </si>
-  <si>
-    <t>TRANSSHIPMENT</t>
-  </si>
-  <si>
     <t>CARRIER</t>
   </si>
   <si>
@@ -106,15 +106,15 @@
     <t>SEGOT</t>
   </si>
   <si>
+    <t>CNSHA</t>
+  </si>
+  <si>
+    <t>ZACPT</t>
+  </si>
+  <si>
     <t>ocean</t>
   </si>
   <si>
-    <t>CNSHA</t>
-  </si>
-  <si>
-    <t>ZACPT</t>
-  </si>
-  <si>
     <t>MSC</t>
   </si>
   <si>
@@ -148,10 +148,7 @@
     <t>Shanghai</t>
   </si>
   <si>
-    <t>PSS</t>
-  </si>
-  <si>
-    <t>Peak Season</t>
+    <t>IMO 2020</t>
   </si>
   <si>
     <t>BAF</t>
@@ -189,7 +186,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -204,34 +201,23 @@
     <font>
       <b/>
       <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -263,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -271,45 +257,25 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -319,15 +285,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,14 +345,14 @@
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
+        <a:latin typeface="calibri"/>
+        <a:ea typeface="calibri"/>
+        <a:cs typeface="calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
+        <a:latin typeface="calibri"/>
+        <a:ea typeface="calibri"/>
+        <a:cs typeface="calibri"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,22 +506,31 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.13"/>
-    <col customWidth="1" min="2" max="2" width="12.38"/>
-    <col customWidth="1" min="3" max="3" width="15.5"/>
-    <col customWidth="1" min="4" max="4" width="17.63"/>
-    <col customWidth="1" min="5" max="5" width="13.75"/>
-    <col customWidth="1" min="6" max="10" width="18.38"/>
-    <col customWidth="1" min="11" max="11" width="14.25"/>
-    <col customWidth="1" min="12" max="12" width="7.75"/>
-    <col customWidth="1" min="13" max="13" width="11.25"/>
-    <col customWidth="1" min="14" max="14" width="12.5"/>
-    <col customWidth="1" min="15" max="15" width="9.88"/>
-    <col customWidth="1" min="16" max="16" width="9.25"/>
-    <col customWidth="1" min="17" max="17" width="10.0"/>
-    <col customWidth="1" min="18" max="18" width="8.75"/>
-    <col customWidth="1" min="19" max="19" width="18.38"/>
-    <col customWidth="1" min="20" max="26" width="7.75"/>
+    <col customWidth="1" min="1" max="1" width="36.5"/>
+    <col customWidth="1" min="2" max="2" width="14.13"/>
+    <col customWidth="1" min="3" max="4" width="18.0"/>
+    <col customWidth="1" min="5" max="5" width="17.5"/>
+    <col customWidth="1" min="6" max="6" width="10.63"/>
+    <col customWidth="1" min="7" max="7" width="16.25"/>
+    <col customWidth="1" min="8" max="8" width="23.25"/>
+    <col customWidth="1" min="9" max="9" width="13.13"/>
+    <col customWidth="1" min="10" max="10" width="22.0"/>
+    <col customWidth="1" min="11" max="11" width="16.63"/>
+    <col customWidth="1" min="12" max="12" width="6.0"/>
+    <col customWidth="1" min="13" max="13" width="9.25"/>
+    <col customWidth="1" min="14" max="14" width="15.75"/>
+    <col customWidth="1" min="15" max="15" width="11.75"/>
+    <col customWidth="1" min="16" max="16" width="11.38"/>
+    <col customWidth="1" min="17" max="17" width="12.13"/>
+    <col customWidth="1" min="18" max="18" width="10.88"/>
+    <col customWidth="1" min="19" max="19" width="20.13"/>
+    <col customWidth="1" min="20" max="20" width="9.0"/>
+    <col customWidth="1" min="21" max="21" width="4.63"/>
+    <col customWidth="1" min="22" max="22" width="10.75"/>
+    <col customWidth="1" min="23" max="23" width="10.25"/>
+    <col customWidth="1" min="24" max="24" width="11.88"/>
+    <col customWidth="1" min="25" max="25" width="12.5"/>
+    <col customWidth="1" min="26" max="26" width="10.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -586,342 +552,342 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>44377.0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="5">
         <v>44560.0</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="10" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="12">
+      <c r="T2" s="3">
         <v>210.0</v>
       </c>
-      <c r="U2" s="12">
+      <c r="U2" s="3">
         <v>210.0</v>
       </c>
-      <c r="V2" s="13">
+      <c r="V2" s="3">
         <v>1.0</v>
       </c>
-      <c r="W2" s="13">
+      <c r="W2" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>44377.0</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="5">
         <v>44560.0</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="9" t="s">
+      <c r="I3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K3" s="8"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="12" t="s">
+      <c r="O3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="12">
+      <c r="S3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="3">
         <v>40.0</v>
       </c>
-      <c r="U3" s="12">
+      <c r="U3" s="3">
         <v>40.0</v>
       </c>
-      <c r="V3" s="13">
+      <c r="V3" s="3">
         <v>1.0</v>
       </c>
-      <c r="W3" s="13">
+      <c r="W3" s="3">
         <v>1.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="5">
         <v>44377.0</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>44560.0</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="R4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T4" s="12">
+      <c r="T4" s="3">
         <v>210.0</v>
       </c>
-      <c r="U4" s="12">
+      <c r="U4" s="3">
         <v>210.0</v>
       </c>
-      <c r="V4" s="13">
+      <c r="V4" s="3">
         <v>1.0</v>
       </c>
-      <c r="W4" s="13">
+      <c r="W4" s="3">
         <v>1.0</v>
       </c>
-      <c r="X4" s="13">
+      <c r="X4" s="3">
         <v>0.0</v>
       </c>
-      <c r="Y4" s="13">
+      <c r="Y4" s="3">
         <v>100.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="5">
         <v>44377.0</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="5">
         <v>44560.0</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11" t="s">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="12" t="s">
+      <c r="N5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P5" s="12" t="s">
+      <c r="P5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="4">
+      <c r="T5" s="3">
         <v>210.0</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="3">
         <v>110.0</v>
       </c>
-      <c r="V5" s="13">
+      <c r="V5" s="3">
         <v>1.0</v>
       </c>
-      <c r="W5" s="13">
+      <c r="W5" s="3">
         <v>1.0</v>
       </c>
-      <c r="X5" s="13">
+      <c r="X5" s="3">
         <v>100.0</v>
       </c>
-      <c r="Y5" s="13">
+      <c r="Y5" s="3">
         <v>500.0</v>
       </c>
     </row>
@@ -948,16 +914,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -966,234 +932,234 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="L1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="15"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12">
         <v>44194.0</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="12">
         <v>44561.0</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="10" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="21">
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="13">
         <v>4330.0</v>
       </c>
-      <c r="W2" s="10">
+      <c r="W2" s="6">
         <v>200.0</v>
       </c>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12">
         <v>44194.0</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="12">
         <v>44561.0</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="11"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="8" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="P3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="Q3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="22">
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="13">
         <v>4660.0</v>
       </c>
-      <c r="W3" s="10">
+      <c r="W3" s="6">
         <v>250.0</v>
       </c>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12">
         <v>44194.0</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="12">
         <v>44561.0</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11" t="s">
+      <c r="J4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="R4" s="11" t="s">
+      <c r="P4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="8"/>
-      <c r="T4" s="8"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="22">
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="13">
         <v>5330.0</v>
       </c>
-      <c r="W4" s="10">
+      <c r="W4" s="6">
         <v>300.0</v>
       </c>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
POL-3143: Insert TransitTimes (#2532)
* POL-3142: gem fixes for apple silicon

* POL-3142: rubocop

* POL-3142: rubocop again

* POL-3143: not inserting yet

* POL-3142: removed debase entirely and locked mimemagic

* POL-3142: debase is most certainly needed

* POL-3143: transit time readded

* POL-3143: mystery

* POL-3143: finally fixed it

* POL-3143: reverted org domain factory change

* POL-3143: rubocop

* POL-3143: spec fixes even if they will arrive in POL-3128

* POL-3143: comments and spec fixes

* POL-3143: flipped order

* POL-3143: rubocop

Co-authored-by: Ajith Kumar <88225952+ajithatimc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/excel/example_pricings.xlsx
+++ b/spec/fixtures/files/excel/example_pricings.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>GROUP_ID</t>
   </si>
@@ -103,9 +103,21 @@
     <t>TEST_GROUP</t>
   </si>
   <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Gothenburg</t>
+  </si>
+  <si>
     <t>SEGOT</t>
   </si>
   <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
     <t>CNSHA</t>
   </si>
   <si>
@@ -134,18 +146,6 @@
   </si>
   <si>
     <t>Ocean Freight</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Gothenburg</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Shanghai</t>
   </si>
   <si>
     <t>IMO 2020</t>
@@ -186,11 +186,12 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -207,6 +208,12 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -214,7 +221,8 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <color theme="1"/>
@@ -249,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -261,14 +269,16 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -277,13 +287,16 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -504,33 +517,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="36.5"/>
-    <col customWidth="1" min="2" max="2" width="14.13"/>
-    <col customWidth="1" min="3" max="4" width="18.0"/>
-    <col customWidth="1" min="5" max="5" width="17.5"/>
-    <col customWidth="1" min="6" max="6" width="10.63"/>
-    <col customWidth="1" min="7" max="7" width="16.25"/>
-    <col customWidth="1" min="8" max="8" width="23.25"/>
-    <col customWidth="1" min="9" max="9" width="13.13"/>
-    <col customWidth="1" min="10" max="10" width="22.0"/>
-    <col customWidth="1" min="11" max="11" width="16.63"/>
-    <col customWidth="1" min="12" max="12" width="6.0"/>
-    <col customWidth="1" min="13" max="13" width="9.25"/>
-    <col customWidth="1" min="14" max="14" width="15.75"/>
-    <col customWidth="1" min="15" max="15" width="11.75"/>
-    <col customWidth="1" min="16" max="16" width="11.38"/>
-    <col customWidth="1" min="17" max="17" width="12.13"/>
-    <col customWidth="1" min="18" max="18" width="10.88"/>
-    <col customWidth="1" min="19" max="19" width="20.13"/>
-    <col customWidth="1" min="20" max="20" width="9.0"/>
-    <col customWidth="1" min="21" max="21" width="4.63"/>
-    <col customWidth="1" min="22" max="22" width="10.75"/>
-    <col customWidth="1" min="23" max="23" width="10.25"/>
-    <col customWidth="1" min="24" max="24" width="11.88"/>
-    <col customWidth="1" min="25" max="25" width="12.5"/>
-    <col customWidth="1" min="26" max="26" width="10.0"/>
+    <col customWidth="1" min="1" max="1" width="41.71"/>
+    <col customWidth="1" min="2" max="2" width="16.14"/>
+    <col customWidth="1" min="3" max="4" width="20.57"/>
+    <col customWidth="1" min="5" max="5" width="20.0"/>
+    <col customWidth="1" min="6" max="6" width="12.14"/>
+    <col customWidth="1" min="7" max="7" width="18.57"/>
+    <col customWidth="1" min="8" max="8" width="26.57"/>
+    <col customWidth="1" min="9" max="9" width="15.0"/>
+    <col customWidth="1" min="10" max="10" width="25.14"/>
+    <col customWidth="1" min="11" max="11" width="19.0"/>
+    <col customWidth="1" min="12" max="12" width="6.86"/>
+    <col customWidth="1" min="13" max="13" width="10.57"/>
+    <col customWidth="1" min="14" max="14" width="18.0"/>
+    <col customWidth="1" min="15" max="15" width="13.43"/>
+    <col customWidth="1" min="16" max="16" width="13.0"/>
+    <col customWidth="1" min="17" max="17" width="13.86"/>
+    <col customWidth="1" min="18" max="18" width="12.43"/>
+    <col customWidth="1" min="19" max="19" width="23.0"/>
+    <col customWidth="1" min="20" max="20" width="10.29"/>
+    <col customWidth="1" min="21" max="21" width="5.29"/>
+    <col customWidth="1" min="22" max="22" width="12.29"/>
+    <col customWidth="1" min="23" max="23" width="11.71"/>
+    <col customWidth="1" min="24" max="24" width="13.57"/>
+    <col customWidth="1" min="25" max="25" width="14.29"/>
+    <col customWidth="1" min="26" max="26" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -623,56 +636,64 @@
       <c r="C2" s="5">
         <v>44377.0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>44560.0</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="J2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="K2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="L2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="M2" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="N2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="3">
+        <v>41</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="8">
         <v>210.0</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="8">
         <v>210.0</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="8">
         <v>1.0</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="8">
         <v>1.0</v>
       </c>
     </row>
@@ -683,61 +704,65 @@
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="9">
         <v>44377.0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>44560.0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="Q3" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="8">
         <v>40.0</v>
       </c>
-      <c r="U3" s="3">
+      <c r="U3" s="8">
         <v>40.0</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="8">
         <v>1.0</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="8">
         <v>1.0</v>
       </c>
     </row>
@@ -748,48 +773,48 @@
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>44377.0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>44560.0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="Q4" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>44</v>
@@ -797,22 +822,22 @@
       <c r="S4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="8">
         <v>210.0</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="8">
         <v>210.0</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="8">
         <v>1.0</v>
       </c>
-      <c r="W4" s="3">
+      <c r="W4" s="8">
         <v>1.0</v>
       </c>
-      <c r="X4" s="3">
+      <c r="X4" s="8">
         <v>0.0</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Y4" s="8">
         <v>100.0</v>
       </c>
     </row>
@@ -823,48 +848,48 @@
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>44377.0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>44560.0</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="Q5" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>44</v>
@@ -878,16 +903,16 @@
       <c r="U5" s="3">
         <v>110.0</v>
       </c>
-      <c r="V5" s="3">
+      <c r="V5" s="8">
         <v>1.0</v>
       </c>
-      <c r="W5" s="3">
+      <c r="W5" s="8">
         <v>1.0</v>
       </c>
-      <c r="X5" s="3">
+      <c r="X5" s="8">
         <v>100.0</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="Y5" s="8">
         <v>500.0</v>
       </c>
     </row>
@@ -907,10 +932,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="5" max="7" width="16.38"/>
-    <col customWidth="1" min="8" max="10" width="22.13"/>
+    <col customWidth="1" min="5" max="7" width="18.71"/>
+    <col customWidth="1" min="8" max="10" width="25.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -920,10 +945,10 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -944,19 +969,19 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="12" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
@@ -977,7 +1002,7 @@
       <c r="U1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="V1" s="12" t="s">
         <v>47</v>
       </c>
       <c r="W1" s="2" t="s">
@@ -985,181 +1010,195 @@
       </c>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-      <c r="Z1" s="6"/>
+      <c r="Z1" s="7"/>
       <c r="AA1" s="2"/>
     </row>
     <row r="2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="14">
         <v>44194.0</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="14">
         <v>44561.0</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="K2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="15">
+        <v>35.0</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="13">
+      <c r="R2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="16">
         <v>4330.0</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2" s="7">
         <v>200.0</v>
       </c>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="6"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14">
         <v>44194.0</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="14">
         <v>44561.0</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="13">
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="16">
         <v>4660.0</v>
       </c>
-      <c r="W3" s="6">
+      <c r="W3" s="7">
         <v>250.0</v>
       </c>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="14">
         <v>44194.0</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="14">
         <v>44561.0</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="13">
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="16">
         <v>5330.0</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="7">
         <v>300.0</v>
       </c>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>